<commit_message>
0312 image, monitor analyzer update
</commit_message>
<xml_diff>
--- a/IoTgateway/Java/AiTESIoTgateway/smartHome_data.xlsx
+++ b/IoTgateway/Java/AiTESIoTgateway/smartHome_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>flowerPot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,12 +78,72 @@
     <t>Robotic Vacuum Cleaner</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.224,127.07.512</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.22,127.07.43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.21,127.07.36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.224,127.07.412</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.24,127.07.212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.28,127.07.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.214,127.07.411</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.45,127.07.223</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.14,127.07.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.220,127.07.107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.224,127.07.232</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.224,127.07.213</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.214,127.07.211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +197,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,15 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M337"/>
+  <dimension ref="A1:O337"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M337"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -453,8 +520,14 @@
       <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="2">
         <v>42933</v>
       </c>
@@ -494,8 +567,14 @@
       <c r="M2" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="1">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2">
         <v>42933.041666666664</v>
       </c>
@@ -535,8 +614,14 @@
       <c r="M3" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="1">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="2">
         <v>42933.083333333336</v>
       </c>
@@ -576,8 +661,14 @@
       <c r="M4" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="1">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="2">
         <v>42933.124999826388</v>
       </c>
@@ -617,8 +708,14 @@
       <c r="M5" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="2">
         <v>42933.166666435187</v>
       </c>
@@ -658,8 +755,14 @@
       <c r="M6" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="1">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="2">
         <v>42933.208333043978</v>
       </c>
@@ -699,8 +802,14 @@
       <c r="M7" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2">
         <v>42933.249999652777</v>
       </c>
@@ -740,8 +849,14 @@
       <c r="M8" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="1">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="2">
         <v>42933.291666261575</v>
       </c>
@@ -781,8 +896,14 @@
       <c r="M9" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="1">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2">
         <v>42933.333332870374</v>
       </c>
@@ -822,8 +943,14 @@
       <c r="M10" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="1">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2">
         <v>42933.374999479165</v>
       </c>
@@ -863,8 +990,14 @@
       <c r="M11" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="1">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="2">
         <v>42933.416666087964</v>
       </c>
@@ -904,8 +1037,14 @@
       <c r="M12" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2">
         <v>42933.458332696762</v>
       </c>
@@ -945,8 +1084,14 @@
       <c r="M13" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="1">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2">
         <v>42933.499999305554</v>
       </c>
@@ -986,8 +1131,14 @@
       <c r="M14" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="1">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="2">
         <v>42933.541665914352</v>
       </c>
@@ -1027,8 +1178,14 @@
       <c r="M15" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="1">
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="2">
         <v>42933.583332523151</v>
       </c>
@@ -1068,8 +1225,14 @@
       <c r="M16" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="1">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="2">
         <v>42933.624999131942</v>
       </c>
@@ -1109,8 +1272,14 @@
       <c r="M17" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="1">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2">
         <v>42933.66666574074</v>
       </c>
@@ -1150,8 +1319,14 @@
       <c r="M18" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="1">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2">
         <v>42933.708332349539</v>
       </c>
@@ -1191,8 +1366,14 @@
       <c r="M19" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2">
         <v>42933.74999895833</v>
       </c>
@@ -1232,8 +1413,14 @@
       <c r="M20" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="1">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="2">
         <v>42933.791665567129</v>
       </c>
@@ -1273,8 +1460,14 @@
       <c r="M21" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="1">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2">
         <v>42933.833332175927</v>
       </c>
@@ -1314,8 +1507,14 @@
       <c r="M22" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="1">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="2">
         <v>42933.874998784719</v>
       </c>
@@ -1355,8 +1554,14 @@
       <c r="M23" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="1">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2">
         <v>42933.916665393517</v>
       </c>
@@ -1396,8 +1601,14 @@
       <c r="M24" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="1">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="2">
         <v>42933.958332002316</v>
       </c>
@@ -1437,8 +1648,14 @@
       <c r="M25" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="1">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2">
         <v>42933.999998611114</v>
       </c>
@@ -1478,8 +1695,14 @@
       <c r="M26" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="1">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="2">
         <v>42934.041665219906</v>
       </c>
@@ -1519,8 +1742,14 @@
       <c r="M27" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>18</v>
+      </c>
+      <c r="O27" s="1">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2">
         <v>42934.083331828704</v>
       </c>
@@ -1560,8 +1789,14 @@
       <c r="M28" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="1">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="2">
         <v>42934.124998437503</v>
       </c>
@@ -1601,8 +1836,14 @@
       <c r="M29" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+      <c r="O29" s="1">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2">
         <v>42934.166665046294</v>
       </c>
@@ -1642,8 +1883,14 @@
       <c r="M30" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="1">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="2">
         <v>42934.208331655092</v>
       </c>
@@ -1683,8 +1930,14 @@
       <c r="M31" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="1">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2">
         <v>42934.249998263891</v>
       </c>
@@ -1724,8 +1977,14 @@
       <c r="M32" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" s="1">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2">
         <v>42934.291664872682</v>
       </c>
@@ -1765,8 +2024,14 @@
       <c r="M33" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" s="1">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2">
         <v>42934.333331481481</v>
       </c>
@@ -1806,8 +2071,14 @@
       <c r="M34" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="1">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="2">
         <v>42934.374998090279</v>
       </c>
@@ -1847,8 +2118,14 @@
       <c r="M35" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>17</v>
+      </c>
+      <c r="O35" s="1">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2">
         <v>42934.416664699071</v>
       </c>
@@ -1888,8 +2165,14 @@
       <c r="M36" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2">
         <v>42934.458331307869</v>
       </c>
@@ -1929,8 +2212,14 @@
       <c r="M37" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>15</v>
+      </c>
+      <c r="O37" s="1">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="2">
         <v>42934.499997916668</v>
       </c>
@@ -1970,8 +2259,11 @@
       <c r="M38" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O38" s="1">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="2">
         <v>42934.541664525466</v>
       </c>
@@ -2011,8 +2303,11 @@
       <c r="M39" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O39" s="1">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="2">
         <v>42934.583331134258</v>
       </c>
@@ -2052,8 +2347,11 @@
       <c r="M40" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O40" s="1">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="2">
         <v>42934.624997743056</v>
       </c>
@@ -2094,7 +2392,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="2">
         <v>42934.666664351855</v>
       </c>
@@ -2135,7 +2433,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" s="2">
         <v>42934.708330960646</v>
       </c>
@@ -2176,7 +2474,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="2">
         <v>42934.749997569445</v>
       </c>
@@ -2217,7 +2515,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" s="2">
         <v>42934.791664178243</v>
       </c>
@@ -2258,7 +2556,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="2">
         <v>42934.833330787034</v>
       </c>
@@ -2299,7 +2597,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="2">
         <v>42934.874997395833</v>
       </c>
@@ -2340,7 +2638,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" s="2">
         <v>42934.916664004631</v>
       </c>
@@ -2381,7 +2679,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="2">
         <v>42934.958330613423</v>
       </c>
@@ -2422,7 +2720,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="2">
         <v>42934.999997222221</v>
       </c>
@@ -2463,7 +2761,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="2">
         <v>42935.04166383102</v>
       </c>
@@ -2504,7 +2802,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="2">
         <v>42935.083330439818</v>
       </c>
@@ -2545,7 +2843,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="2">
         <v>42935.12499704861</v>
       </c>
@@ -2586,7 +2884,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="2">
         <v>42935.166663657408</v>
       </c>
@@ -2627,7 +2925,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="2">
         <v>42935.208330266207</v>
       </c>
@@ -2668,7 +2966,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="2">
         <v>42935.249996874998</v>
       </c>
@@ -2709,7 +3007,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="2">
         <v>42935.291663483797</v>
       </c>
@@ -2750,7 +3048,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="2">
         <v>42935.333330092595</v>
       </c>
@@ -2791,7 +3089,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="2">
         <v>42935.374996701386</v>
       </c>
@@ -2832,7 +3130,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="2">
         <v>42935.416663310185</v>
       </c>
@@ -2873,7 +3171,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="2">
         <v>42935.458329918984</v>
       </c>
@@ -2914,7 +3212,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="2">
         <v>42935.499996527775</v>
       </c>
@@ -2955,7 +3253,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="2">
         <v>42935.541663136573</v>
       </c>
@@ -2996,7 +3294,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="2">
         <v>42935.583329745372</v>
       </c>
@@ -3037,7 +3335,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="2">
         <v>42935.624996354163</v>
       </c>
@@ -3078,7 +3376,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="2">
         <v>42935.666662962962</v>
       </c>
@@ -3119,7 +3417,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="2">
         <v>42935.70832957176</v>
       </c>
@@ -3160,7 +3458,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="2">
         <v>42935.749996180559</v>
       </c>
@@ -3201,7 +3499,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="2">
         <v>42935.79166278935</v>
       </c>
@@ -3242,7 +3540,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="2">
         <v>42935.833329398149</v>
       </c>
@@ -3283,7 +3581,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="2">
         <v>42935.874996006947</v>
       </c>
@@ -3324,7 +3622,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="2">
         <v>42935.916662615738</v>
       </c>
@@ -3365,7 +3663,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="2">
         <v>42935.958329224537</v>
       </c>
@@ -3406,7 +3704,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="2">
         <v>42935.999995833336</v>
       </c>
@@ -3447,7 +3745,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="2">
         <v>42936.041662442127</v>
       </c>
@@ -3488,7 +3786,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="2">
         <v>42936.083329050925</v>
       </c>
@@ -3529,7 +3827,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" s="2">
         <v>42936.124995659724</v>
       </c>
@@ -3570,7 +3868,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" s="2">
         <v>42936.166662268515</v>
       </c>
@@ -3611,7 +3909,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" s="2">
         <v>42936.208328877314</v>
       </c>
@@ -3652,7 +3950,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" s="2">
         <v>42936.249995486112</v>
       </c>
@@ -3693,7 +3991,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13">
       <c r="A81" s="2">
         <v>42936.291662094911</v>
       </c>
@@ -3734,7 +4032,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" s="2">
         <v>42936.333328703702</v>
       </c>
@@ -3775,7 +4073,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" s="2">
         <v>42936.374995312501</v>
       </c>
@@ -3816,7 +4114,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" s="2">
         <v>42936.416661921299</v>
       </c>
@@ -3857,7 +4155,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13">
       <c r="A85" s="2">
         <v>42936.458328530091</v>
       </c>
@@ -3898,7 +4196,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13">
       <c r="A86" s="2">
         <v>42936.499995138889</v>
       </c>
@@ -3939,7 +4237,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="A87" s="2">
         <v>42936.541661747688</v>
       </c>
@@ -3980,7 +4278,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="A88" s="2">
         <v>42936.583328356479</v>
       </c>
@@ -4021,7 +4319,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="A89" s="2">
         <v>42936.624994965277</v>
       </c>
@@ -4062,7 +4360,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" s="2">
         <v>42936.666661574076</v>
       </c>
@@ -4103,7 +4401,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" s="2">
         <v>42936.708328182867</v>
       </c>
@@ -4144,7 +4442,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" s="2">
         <v>42936.749994791666</v>
       </c>
@@ -4185,7 +4483,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" s="2">
         <v>42936.791661400464</v>
       </c>
@@ -4226,7 +4524,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="A94" s="2">
         <v>42936.833328009256</v>
       </c>
@@ -4267,7 +4565,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13">
       <c r="A95" s="2">
         <v>42936.874994618054</v>
       </c>
@@ -4308,7 +4606,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="2">
         <v>42936.916661226853</v>
       </c>
@@ -4349,7 +4647,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13">
       <c r="A97" s="2">
         <v>42936.958327835651</v>
       </c>
@@ -4390,7 +4688,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13">
       <c r="A98" s="2">
         <v>42936.999994444443</v>
       </c>
@@ -4431,7 +4729,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13">
       <c r="A99" s="2">
         <v>42937.041661053241</v>
       </c>
@@ -4472,7 +4770,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13">
       <c r="A100" s="2">
         <v>42937.08332766204</v>
       </c>
@@ -4513,7 +4811,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13">
       <c r="A101" s="2">
         <v>42937.124994270831</v>
       </c>
@@ -4554,7 +4852,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13">
       <c r="A102" s="2">
         <v>42937.166666666664</v>
       </c>
@@ -4595,7 +4893,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13">
       <c r="A103" s="2">
         <v>42937.208339004632</v>
       </c>
@@ -4636,7 +4934,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13">
       <c r="A104" s="2">
         <v>42937.250011400465</v>
       </c>
@@ -4677,7 +4975,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13">
       <c r="A105" s="2">
         <v>42937.291683796298</v>
       </c>
@@ -4718,7 +5016,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13">
       <c r="A106" s="2">
         <v>42937.333356192132</v>
       </c>
@@ -4759,7 +5057,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13">
       <c r="A107" s="2">
         <v>42937.375028587965</v>
       </c>
@@ -4800,7 +5098,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13">
       <c r="A108" s="2">
         <v>42937.416700983798</v>
       </c>
@@ -4841,7 +5139,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13">
       <c r="A109" s="2">
         <v>42937.458373379632</v>
       </c>
@@ -4882,7 +5180,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13">
       <c r="A110" s="2">
         <v>42937.500045775465</v>
       </c>
@@ -4923,7 +5221,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13">
       <c r="A111" s="2">
         <v>42937.541718171298</v>
       </c>
@@ -4964,7 +5262,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13">
       <c r="A112" s="2">
         <v>42937.583390567132</v>
       </c>
@@ -5005,7 +5303,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13">
       <c r="A113" s="2">
         <v>42937.625062962965</v>
       </c>
@@ -5046,7 +5344,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13">
       <c r="A114" s="2">
         <v>42937.666735358798</v>
       </c>
@@ -5087,7 +5385,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13">
       <c r="A115" s="2">
         <v>42937.708407754631</v>
       </c>
@@ -5128,7 +5426,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13">
       <c r="A116" s="2">
         <v>42937.750080150465</v>
       </c>
@@ -5169,7 +5467,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13">
       <c r="A117" s="2">
         <v>42937.791752546298</v>
       </c>
@@ -5210,7 +5508,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13">
       <c r="A118" s="2">
         <v>42937.833424942131</v>
       </c>
@@ -5251,7 +5549,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13">
       <c r="A119" s="2">
         <v>42937.875097337965</v>
       </c>
@@ -5292,7 +5590,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13">
       <c r="A120" s="2">
         <v>42937.916769733798</v>
       </c>
@@ -5333,7 +5631,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13">
       <c r="A121" s="2">
         <v>42937.958442129631</v>
       </c>
@@ -5374,7 +5672,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13">
       <c r="A122" s="2">
         <v>42938.000114525465</v>
       </c>
@@ -5415,7 +5713,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13">
       <c r="A123" s="2">
         <v>42938.041786921298</v>
       </c>
@@ -5456,7 +5754,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13">
       <c r="A124" s="2">
         <v>42938.083459317131</v>
       </c>
@@ -5497,7 +5795,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13">
       <c r="A125" s="2">
         <v>42938.125131712965</v>
       </c>
@@ -5538,7 +5836,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13">
       <c r="A126" s="2">
         <v>42938.166804108798</v>
       </c>
@@ -5579,7 +5877,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13">
       <c r="A127" s="2">
         <v>42938.208476504631</v>
       </c>
@@ -5620,7 +5918,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13">
       <c r="A128" s="2">
         <v>42938.250148900464</v>
       </c>
@@ -5661,7 +5959,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13">
       <c r="A129" s="2">
         <v>42938.291821296298</v>
       </c>
@@ -5702,7 +6000,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13">
       <c r="A130" s="2">
         <v>42938.333493692131</v>
       </c>
@@ -5743,7 +6041,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13">
       <c r="A131" s="2">
         <v>42938.375166087964</v>
       </c>
@@ -5784,7 +6082,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13">
       <c r="A132" s="2">
         <v>42938.416838483798</v>
       </c>
@@ -5825,7 +6123,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13">
       <c r="A133" s="2">
         <v>42938.458510879631</v>
       </c>
@@ -5866,7 +6164,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13">
       <c r="A134" s="2">
         <v>42938.500183275464</v>
       </c>
@@ -5907,7 +6205,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13">
       <c r="A135" s="2">
         <v>42938.541855671298</v>
       </c>
@@ -5948,7 +6246,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13">
       <c r="A136" s="2">
         <v>42938.583528067131</v>
       </c>
@@ -5989,7 +6287,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13">
       <c r="A137" s="2">
         <v>42938.625200462964</v>
       </c>
@@ -6030,7 +6328,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13">
       <c r="A138" s="2">
         <v>42938.666872858797</v>
       </c>
@@ -6071,7 +6369,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13">
       <c r="A139" s="2">
         <v>42938.708545254631</v>
       </c>
@@ -6112,7 +6410,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13">
       <c r="A140" s="2">
         <v>42938.750217650464</v>
       </c>
@@ -6153,7 +6451,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13">
       <c r="A141" s="2">
         <v>42938.791890046297</v>
       </c>
@@ -6194,7 +6492,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13">
       <c r="A142" s="2">
         <v>42938.833562442131</v>
       </c>
@@ -6235,7 +6533,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13">
       <c r="A143" s="2">
         <v>42938.875234837964</v>
       </c>
@@ -6276,7 +6574,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13">
       <c r="A144" s="2">
         <v>42938.916907233797</v>
       </c>
@@ -6317,7 +6615,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13">
       <c r="A145" s="2">
         <v>42938.958579629631</v>
       </c>
@@ -6358,7 +6656,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13">
       <c r="A146" s="2">
         <v>42939.000252025464</v>
       </c>
@@ -6399,7 +6697,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13">
       <c r="A147" s="2">
         <v>42939.041924421297</v>
       </c>
@@ -6440,7 +6738,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13">
       <c r="A148" s="2">
         <v>42939.08359681713</v>
       </c>
@@ -6481,7 +6779,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13">
       <c r="A149" s="2">
         <v>42939.125269212964</v>
       </c>
@@ -6522,7 +6820,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13">
       <c r="A150" s="2">
         <v>42939.166941608797</v>
       </c>
@@ -6563,7 +6861,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13">
       <c r="A151" s="2">
         <v>42939.20861400463</v>
       </c>
@@ -6604,7 +6902,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13">
       <c r="A152" s="2">
         <v>42939.250286400464</v>
       </c>
@@ -6645,7 +6943,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13">
       <c r="A153" s="2">
         <v>42939.291958796297</v>
       </c>
@@ -6686,7 +6984,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13">
       <c r="A154" s="2">
         <v>42939.33363119213</v>
       </c>
@@ -6727,7 +7025,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13">
       <c r="A155" s="2">
         <v>42939.375303587964</v>
       </c>
@@ -6768,7 +7066,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13">
       <c r="A156" s="2">
         <v>42939.416975983797</v>
       </c>
@@ -6809,7 +7107,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13">
       <c r="A157" s="2">
         <v>42939.45864837963</v>
       </c>
@@ -6850,7 +7148,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13">
       <c r="A158" s="2">
         <v>42939.500320775463</v>
       </c>
@@ -6891,7 +7189,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13">
       <c r="A159" s="2">
         <v>42939.541993171297</v>
       </c>
@@ -6932,7 +7230,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13">
       <c r="A160" s="2">
         <v>42939.58366556713</v>
       </c>
@@ -6973,7 +7271,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13">
       <c r="A161" s="2">
         <v>42939.625337962963</v>
       </c>
@@ -7014,7 +7312,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13">
       <c r="A162" s="2">
         <v>42939.667010358797</v>
       </c>
@@ -7055,7 +7353,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13">
       <c r="A163" s="2">
         <v>42939.70868275463</v>
       </c>
@@ -7096,7 +7394,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13">
       <c r="A164" s="2">
         <v>42939.750355150463</v>
       </c>
@@ -7137,7 +7435,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13">
       <c r="A165" s="2">
         <v>42939.792027546297</v>
       </c>
@@ -7178,7 +7476,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13">
       <c r="A166" s="2">
         <v>42939.83369994213</v>
       </c>
@@ -7219,7 +7517,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13">
       <c r="A167" s="2">
         <v>42939.875372337963</v>
       </c>
@@ -7260,7 +7558,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13">
       <c r="A168" s="2">
         <v>42939.917044733797</v>
       </c>
@@ -7301,7 +7599,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13">
       <c r="A169" s="2">
         <v>42939.95871712963</v>
       </c>
@@ -7342,7 +7640,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13">
       <c r="A170" s="2">
         <v>42940.000389525463</v>
       </c>
@@ -7383,7 +7681,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13">
       <c r="A171" s="2">
         <v>42940.042061921296</v>
       </c>
@@ -7424,7 +7722,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13">
       <c r="A172" s="2">
         <v>42940.08373431713</v>
       </c>
@@ -7465,7 +7763,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13">
       <c r="A173" s="2">
         <v>42940.125406712963</v>
       </c>
@@ -7506,7 +7804,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13">
       <c r="A174" s="2">
         <v>42940.167079108796</v>
       </c>
@@ -7547,7 +7845,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13">
       <c r="A175" s="2">
         <v>42940.20875150463</v>
       </c>
@@ -7588,7 +7886,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13">
       <c r="A176" s="2">
         <v>42940.250423900463</v>
       </c>
@@ -7629,7 +7927,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13">
       <c r="A177" s="2">
         <v>42940.292096296296</v>
       </c>
@@ -7670,7 +7968,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13">
       <c r="A178" s="2">
         <v>42940.33376869213</v>
       </c>
@@ -7711,7 +8009,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13">
       <c r="A179" s="2">
         <v>42940.37544103009</v>
       </c>
@@ -7752,7 +8050,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13">
       <c r="A180" s="2">
         <v>42940.417113425923</v>
       </c>
@@ -7793,7 +8091,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13">
       <c r="A181" s="2">
         <v>42940.458785821756</v>
       </c>
@@ -7834,7 +8132,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13">
       <c r="A182" s="2">
         <v>42940.50045821759</v>
       </c>
@@ -7875,7 +8173,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13">
       <c r="A183" s="2">
         <v>42940.542130613423</v>
       </c>
@@ -7916,7 +8214,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13">
       <c r="A184" s="2">
         <v>42940.583803009256</v>
       </c>
@@ -7957,7 +8255,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13">
       <c r="A185" s="2">
         <v>42940.62547540509</v>
       </c>
@@ -7998,7 +8296,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13">
       <c r="A186" s="2">
         <v>42940.667147800923</v>
       </c>
@@ -8039,7 +8337,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13">
       <c r="A187" s="2">
         <v>42940.708820196756</v>
       </c>
@@ -8080,7 +8378,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13">
       <c r="A188" s="2">
         <v>42940.75049259259</v>
       </c>
@@ -8121,7 +8419,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13">
       <c r="A189" s="2">
         <v>42940.792164988423</v>
       </c>
@@ -8162,7 +8460,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13">
       <c r="A190" s="2">
         <v>42940.833837384256</v>
       </c>
@@ -8203,7 +8501,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13">
       <c r="A191" s="2">
         <v>42940.875509780089</v>
       </c>
@@ -8244,7 +8542,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13">
       <c r="A192" s="2">
         <v>42940.917182175923</v>
       </c>
@@ -8285,7 +8583,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13">
       <c r="A193" s="2">
         <v>42940.95885451389</v>
       </c>
@@ -8326,7 +8624,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13">
       <c r="A194" s="2">
         <v>42941.000526909724</v>
       </c>
@@ -8367,7 +8665,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13">
       <c r="A195" s="2">
         <v>42941.042199305557</v>
       </c>
@@ -8408,7 +8706,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13">
       <c r="A196" s="2">
         <v>42941.08387170139</v>
       </c>
@@ -8449,7 +8747,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13">
       <c r="A197" s="2">
         <v>42941.125544097224</v>
       </c>
@@ -8490,7 +8788,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13">
       <c r="A198" s="2">
         <v>42941.167216493057</v>
       </c>
@@ -8531,7 +8829,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13">
       <c r="A199" s="2">
         <v>42941.20888888889</v>
       </c>
@@ -8572,7 +8870,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13">
       <c r="A200" s="2">
         <v>42941.250561284724</v>
       </c>
@@ -8613,7 +8911,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13">
       <c r="A201" s="2">
         <v>42941.292233680557</v>
       </c>
@@ -8654,7 +8952,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13">
       <c r="A202" s="2">
         <v>42941.33390607639</v>
       </c>
@@ -8695,7 +8993,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13">
       <c r="A203" s="2">
         <v>42941.375578472223</v>
       </c>
@@ -8736,7 +9034,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13">
       <c r="A204" s="2">
         <v>42941.417250868057</v>
       </c>
@@ -8777,7 +9075,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13">
       <c r="A205" s="2">
         <v>42941.45892326389</v>
       </c>
@@ -8818,7 +9116,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13">
       <c r="A206" s="2">
         <v>42941.500595659723</v>
       </c>
@@ -8859,7 +9157,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13">
       <c r="A207" s="2">
         <v>42941.542268055557</v>
       </c>
@@ -8900,7 +9198,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13">
       <c r="A208" s="2">
         <v>42941.58394045139</v>
       </c>
@@ -8941,7 +9239,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13">
       <c r="A209" s="2">
         <v>42941.625612847223</v>
       </c>
@@ -8982,7 +9280,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13">
       <c r="A210" s="2">
         <v>42941.667285243057</v>
       </c>
@@ -9023,7 +9321,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13">
       <c r="A211" s="2">
         <v>42941.70895763889</v>
       </c>
@@ -9064,7 +9362,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13">
       <c r="A212" s="2">
         <v>42941.750630034723</v>
       </c>
@@ -9105,7 +9403,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13">
       <c r="A213" s="2">
         <v>42941.792302430556</v>
       </c>
@@ -9146,7 +9444,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13">
       <c r="A214" s="2">
         <v>42941.83397482639</v>
       </c>
@@ -9187,7 +9485,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13">
       <c r="A215" s="2">
         <v>42941.875647222223</v>
       </c>
@@ -9228,7 +9526,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13">
       <c r="A216" s="2">
         <v>42941.917319618056</v>
       </c>
@@ -9269,7 +9567,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13">
       <c r="A217" s="2">
         <v>42941.958993055552</v>
       </c>
@@ -9310,7 +9608,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13">
       <c r="A218" s="2">
         <v>42942.000664409723</v>
       </c>
@@ -9351,7 +9649,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13">
       <c r="A219" s="2">
         <v>42942.042336805556</v>
       </c>
@@ -9392,7 +9690,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13">
       <c r="A220" s="2">
         <v>42942.08400920139</v>
       </c>
@@ -9433,7 +9731,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13">
       <c r="A221" s="2">
         <v>42942.125681597223</v>
       </c>
@@ -9474,7 +9772,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13">
       <c r="A222" s="2">
         <v>42942.166666666664</v>
       </c>
@@ -9515,7 +9813,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13">
       <c r="A223" s="2">
         <v>42942.208333333336</v>
       </c>
@@ -9556,7 +9854,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13">
       <c r="A224" s="2">
         <v>42942.25</v>
       </c>
@@ -9597,7 +9895,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13">
       <c r="A225" s="2">
         <v>42942.291666666664</v>
       </c>
@@ -9638,7 +9936,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13">
       <c r="A226" s="2">
         <v>42942.333333333336</v>
       </c>
@@ -9679,7 +9977,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13">
       <c r="A227" s="2">
         <v>42942.375</v>
       </c>
@@ -9720,7 +10018,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13">
       <c r="A228" s="2">
         <v>42942.416666666664</v>
       </c>
@@ -9761,7 +10059,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13">
       <c r="A229" s="2">
         <v>42942.458333333336</v>
       </c>
@@ -9802,7 +10100,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13">
       <c r="A230" s="2">
         <v>42942.5</v>
       </c>
@@ -9843,7 +10141,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13">
       <c r="A231" s="2">
         <v>42942.541666666664</v>
       </c>
@@ -9884,7 +10182,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13">
       <c r="A232" s="2">
         <v>42942.58333321759</v>
       </c>
@@ -9925,7 +10223,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13">
       <c r="A233" s="2">
         <v>42942.624999826388</v>
       </c>
@@ -9966,7 +10264,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13">
       <c r="A234" s="2">
         <v>42942.666666435187</v>
       </c>
@@ -10007,7 +10305,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13">
       <c r="A235" s="2">
         <v>42942.708333043978</v>
       </c>
@@ -10048,7 +10346,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13">
       <c r="A236" s="2">
         <v>42942.749999652777</v>
       </c>
@@ -10089,7 +10387,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13">
       <c r="A237" s="2">
         <v>42942.791666261575</v>
       </c>
@@ -10130,7 +10428,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13">
       <c r="A238" s="2">
         <v>42942.833332870374</v>
       </c>
@@ -10171,7 +10469,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13">
       <c r="A239" s="2">
         <v>42942.874999479165</v>
       </c>
@@ -10212,7 +10510,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13">
       <c r="A240" s="2">
         <v>42942.916666087964</v>
       </c>
@@ -10253,7 +10551,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13">
       <c r="A241" s="2">
         <v>42942.958332696762</v>
       </c>
@@ -10294,7 +10592,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13">
       <c r="A242" s="2">
         <v>42942.999999305554</v>
       </c>
@@ -10335,7 +10633,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13">
       <c r="A243" s="2">
         <v>42943.041665914352</v>
       </c>
@@ -10376,7 +10674,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13">
       <c r="A244" s="2">
         <v>42943.083332523151</v>
       </c>
@@ -10417,7 +10715,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13">
       <c r="A245" s="2">
         <v>42943.124999131942</v>
       </c>
@@ -10458,7 +10756,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13">
       <c r="A246" s="2">
         <v>42943.16666574074</v>
       </c>
@@ -10499,7 +10797,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13">
       <c r="A247" s="2">
         <v>42943.208332349539</v>
       </c>
@@ -10540,7 +10838,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13">
       <c r="A248" s="2">
         <v>42943.24999895833</v>
       </c>
@@ -10581,7 +10879,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13">
       <c r="A249" s="2">
         <v>42943.291665567129</v>
       </c>
@@ -10622,7 +10920,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13">
       <c r="A250" s="2">
         <v>42943.333332175927</v>
       </c>
@@ -10663,7 +10961,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13">
       <c r="A251" s="2">
         <v>42943.374998784719</v>
       </c>
@@ -10704,7 +11002,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13">
       <c r="A252" s="2">
         <v>42943.416665393517</v>
       </c>
@@ -10745,7 +11043,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13">
       <c r="A253" s="2">
         <v>42943.458332002316</v>
       </c>
@@ -10786,7 +11084,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13">
       <c r="A254" s="2">
         <v>42943.499998611114</v>
       </c>
@@ -10827,7 +11125,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13">
       <c r="A255" s="2">
         <v>42943.541665219906</v>
       </c>
@@ -10868,7 +11166,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13">
       <c r="A256" s="2">
         <v>42943.583331828704</v>
       </c>
@@ -10909,7 +11207,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13">
       <c r="A257" s="2">
         <v>42943.624998437503</v>
       </c>
@@ -10950,7 +11248,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13">
       <c r="A258" s="2">
         <v>42943.666665046294</v>
       </c>
@@ -10991,7 +11289,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13">
       <c r="A259" s="2">
         <v>42943.708331655092</v>
       </c>
@@ -11032,7 +11330,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13">
       <c r="A260" s="2">
         <v>42943.749998263891</v>
       </c>
@@ -11073,7 +11371,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13">
       <c r="A261" s="2">
         <v>42943.791664872682</v>
       </c>
@@ -11114,7 +11412,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13">
       <c r="A262" s="2">
         <v>42943.833331481481</v>
       </c>
@@ -11155,7 +11453,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13">
       <c r="A263" s="2">
         <v>42943.874998090279</v>
       </c>
@@ -11196,7 +11494,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13">
       <c r="A264" s="2">
         <v>42943.916664699071</v>
       </c>
@@ -11237,7 +11535,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13">
       <c r="A265" s="2">
         <v>42943.958331307869</v>
       </c>
@@ -11278,7 +11576,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13">
       <c r="A266" s="2">
         <v>42943.999997916668</v>
       </c>
@@ -11319,7 +11617,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13">
       <c r="A267" s="2">
         <v>42944.041664525466</v>
       </c>
@@ -11360,7 +11658,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13">
       <c r="A268" s="2">
         <v>42944.083331134258</v>
       </c>
@@ -11401,7 +11699,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13">
       <c r="A269" s="2">
         <v>42944.124997743056</v>
       </c>
@@ -11442,7 +11740,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13">
       <c r="A270" s="2">
         <v>42944.166664351855</v>
       </c>
@@ -11483,7 +11781,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13">
       <c r="A271" s="2">
         <v>42944.208330960646</v>
       </c>
@@ -11524,7 +11822,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13">
       <c r="A272" s="2">
         <v>42944.25</v>
       </c>
@@ -11565,7 +11863,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13">
       <c r="A273" s="2">
         <v>42944.291664178243</v>
       </c>
@@ -11606,7 +11904,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13">
       <c r="A274" s="2">
         <v>42944.333328356479</v>
       </c>
@@ -11647,7 +11945,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13">
       <c r="A275" s="2">
         <v>42944.375</v>
       </c>
@@ -11688,7 +11986,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13">
       <c r="A276" s="2">
         <v>42944.416666666664</v>
       </c>
@@ -11729,7 +12027,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13">
       <c r="A277" s="2">
         <v>42944.458333333336</v>
       </c>
@@ -11770,7 +12068,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13">
       <c r="A278" s="2">
         <v>42944.5</v>
       </c>
@@ -11811,7 +12109,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13">
       <c r="A279" s="2">
         <v>42944.541666666664</v>
       </c>
@@ -11852,7 +12150,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13">
       <c r="A280" s="2">
         <v>42944.58333321759</v>
       </c>
@@ -11893,7 +12191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13">
       <c r="A281" s="2">
         <v>42944.624999826388</v>
       </c>
@@ -11934,7 +12232,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13">
       <c r="A282" s="2">
         <v>42944.666666435187</v>
       </c>
@@ -11975,7 +12273,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13">
       <c r="A283" s="2">
         <v>42944.708333043978</v>
       </c>
@@ -12016,7 +12314,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13">
       <c r="A284" s="2">
         <v>42944.749999652777</v>
       </c>
@@ -12057,7 +12355,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13">
       <c r="A285" s="2">
         <v>42944.791666261575</v>
       </c>
@@ -12098,7 +12396,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13">
       <c r="A286" s="2">
         <v>42944.833332870374</v>
       </c>
@@ -12139,7 +12437,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13">
       <c r="A287" s="2">
         <v>42944.874999479165</v>
       </c>
@@ -12180,7 +12478,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13">
       <c r="A288" s="2">
         <v>42944.916666087964</v>
       </c>
@@ -12221,7 +12519,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13">
       <c r="A289" s="2">
         <v>42944.958332696762</v>
       </c>
@@ -12262,7 +12560,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13">
       <c r="A290" s="2">
         <v>42944.999999305554</v>
       </c>
@@ -12303,7 +12601,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13">
       <c r="A291" s="2">
         <v>42945.041666666664</v>
       </c>
@@ -12344,7 +12642,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13">
       <c r="A292" s="2">
         <v>42945.083333333336</v>
       </c>
@@ -12385,7 +12683,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13">
       <c r="A293" s="2">
         <v>42945.125</v>
       </c>
@@ -12426,7 +12724,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13">
       <c r="A294" s="2">
         <v>42945.166666666664</v>
       </c>
@@ -12467,7 +12765,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13">
       <c r="A295" s="2">
         <v>42945.208333333336</v>
       </c>
@@ -12508,7 +12806,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13">
       <c r="A296" s="2">
         <v>42945.25</v>
       </c>
@@ -12549,7 +12847,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13">
       <c r="A297" s="2">
         <v>42945.291666666664</v>
       </c>
@@ -12590,7 +12888,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13">
       <c r="A298" s="2">
         <v>42945.333333333336</v>
       </c>
@@ -12631,7 +12929,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13">
       <c r="A299" s="2">
         <v>42945.375</v>
       </c>
@@ -12672,7 +12970,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13">
       <c r="A300" s="2">
         <v>42945.416666666664</v>
       </c>
@@ -12713,7 +13011,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13">
       <c r="A301" s="2">
         <v>42945.458333333336</v>
       </c>
@@ -12754,7 +13052,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13">
       <c r="A302" s="2">
         <v>42945.5</v>
       </c>
@@ -12795,7 +13093,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13">
       <c r="A303" s="2">
         <v>42945.541666666664</v>
       </c>
@@ -12836,7 +13134,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13">
       <c r="A304" s="2">
         <v>42945.583333333336</v>
       </c>
@@ -12877,7 +13175,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13">
       <c r="A305" s="2">
         <v>42945.625</v>
       </c>
@@ -12918,7 +13216,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13">
       <c r="A306" s="2">
         <v>42945.666666666664</v>
       </c>
@@ -12959,7 +13257,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13">
       <c r="A307" s="2">
         <v>42945.708333333336</v>
       </c>
@@ -13000,7 +13298,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13">
       <c r="A308" s="2">
         <v>42945.75</v>
       </c>
@@ -13041,7 +13339,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13">
       <c r="A309" s="2">
         <v>42945.791666666664</v>
       </c>
@@ -13082,7 +13380,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13">
       <c r="A310" s="2">
         <v>42945.833333333336</v>
       </c>
@@ -13123,7 +13421,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13">
       <c r="A311" s="2">
         <v>42945.875</v>
       </c>
@@ -13164,7 +13462,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13">
       <c r="A312" s="2">
         <v>42945.916666666664</v>
       </c>
@@ -13205,7 +13503,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13">
       <c r="A313" s="2">
         <v>42945.958333333336</v>
       </c>
@@ -13246,7 +13544,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13">
       <c r="A314" s="2">
         <v>42946</v>
       </c>
@@ -13287,7 +13585,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13">
       <c r="A315" s="2">
         <v>42946.041666666664</v>
       </c>
@@ -13328,7 +13626,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13">
       <c r="A316" s="2">
         <v>42946.083333333336</v>
       </c>
@@ -13369,7 +13667,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13">
       <c r="A317" s="2">
         <v>42946.125</v>
       </c>
@@ -13410,7 +13708,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13">
       <c r="A318" s="2">
         <v>42946.166666666664</v>
       </c>
@@ -13451,7 +13749,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13">
       <c r="A319" s="2">
         <v>42946.208333333336</v>
       </c>
@@ -13492,7 +13790,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13">
       <c r="A320" s="2">
         <v>42946.25</v>
       </c>
@@ -13533,7 +13831,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13">
       <c r="A321" s="2">
         <v>42946.291666666664</v>
       </c>
@@ -13574,7 +13872,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13">
       <c r="A322" s="2">
         <v>42946.333333333336</v>
       </c>
@@ -13615,7 +13913,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13">
       <c r="A323" s="2">
         <v>42946.375</v>
       </c>
@@ -13656,7 +13954,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13">
       <c r="A324" s="2">
         <v>42946.416666666664</v>
       </c>
@@ -13697,7 +13995,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13">
       <c r="A325" s="2">
         <v>42946.458333333336</v>
       </c>
@@ -13738,7 +14036,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13">
       <c r="A326" s="2">
         <v>42946.5</v>
       </c>
@@ -13779,7 +14077,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13">
       <c r="A327" s="2">
         <v>42946.541666666664</v>
       </c>
@@ -13820,7 +14118,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13">
       <c r="A328" s="2">
         <v>42946.583333333336</v>
       </c>
@@ -13861,7 +14159,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13">
       <c r="A329" s="2">
         <v>42946.625</v>
       </c>
@@ -13902,7 +14200,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13">
       <c r="A330" s="2">
         <v>42946.666666666664</v>
       </c>
@@ -13943,7 +14241,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13">
       <c r="A331" s="2">
         <v>42946.708333333336</v>
       </c>
@@ -13984,7 +14282,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13">
       <c r="A332" s="2">
         <v>42946.75</v>
       </c>
@@ -14025,7 +14323,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13">
       <c r="A333" s="2">
         <v>42946.791666666664</v>
       </c>
@@ -14066,7 +14364,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13">
       <c r="A334" s="2">
         <v>42946.833333333336</v>
       </c>
@@ -14107,7 +14405,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13">
       <c r="A335" s="2">
         <v>42946.875</v>
       </c>
@@ -14148,7 +14446,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13">
       <c r="A336" s="2">
         <v>42946.916666666664</v>
       </c>
@@ -14189,7 +14487,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13">
       <c r="A337" s="2">
         <v>42946.958333333336</v>
       </c>
@@ -14233,5 +14531,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
iot Gateway Device connection management impl, AiTES log add
</commit_message>
<xml_diff>
--- a/IoTgateway/Java/AiTESIoTgateway/smartHome_data.xlsx
+++ b/IoTgateway/Java/AiTESIoTgateway/smartHome_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="37540" yWindow="3780" windowWidth="27320" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>flowerPot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,55 +87,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.224,127.07.512</t>
+    <t>37.19.24.413:127.07.43.44</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.22,127.07.43</t>
+    <t>37.19.24.416:127.07.43.44</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.21,127.07.36</t>
+    <t>37.19.24.420:127.07.43.46</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.224,127.07.412</t>
+    <t>37.19.24.415:127.07.43.45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.24,127.07.212</t>
+    <t>37.19.24.416:127.07.43.46</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.28,127.07.11</t>
+    <t>37.19.24.422:127.07.43.45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.214,127.07.411</t>
+    <t>37.19.24.414:127.07.43.47</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.45,127.07.223</t>
+    <t>37.19.24.416:127.07.43.48</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.14,127.07.22</t>
+    <t>37.19.24.454:127.07.43.86</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.220,127.07.107</t>
+    <t>37.19.24.564:127.07.43.134</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.224,127.07.232</t>
+    <t>37.19.26.434:127.07.44.167</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.224,127.07.213</t>
+    <t>37.19.56.556:127.07.74.714</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37.19.214,127.07.211</t>
+    <t>37.19.43.764:127.07.214.213</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.144.532:127.07.46.532</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.364.124:127.07.534.634</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.214.643:127.07.334.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.214.643:127.07.334.42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.21.865:127.07.43.412</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.22.132:127.07.48.234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.25.241:127.07.42.234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37.19.62.134:127.07.54.122</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -470,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -567,7 +599,7 @@
       <c r="M2" s="1">
         <v>180</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="1">
@@ -614,8 +646,8 @@
       <c r="M3" s="1">
         <v>180</v>
       </c>
-      <c r="N3" t="s">
-        <v>18</v>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="O3" s="1">
         <v>23.6</v>
@@ -661,8 +693,8 @@
       <c r="M4" s="1">
         <v>180</v>
       </c>
-      <c r="N4" t="s">
-        <v>19</v>
+      <c r="N4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="O4" s="1">
         <v>23.4</v>
@@ -708,8 +740,8 @@
       <c r="M5" s="1">
         <v>180</v>
       </c>
-      <c r="N5" t="s">
-        <v>20</v>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="O5" s="1">
         <v>23.4</v>
@@ -755,8 +787,8 @@
       <c r="M6" s="1">
         <v>180</v>
       </c>
-      <c r="N6" t="s">
-        <v>21</v>
+      <c r="N6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="O6" s="1">
         <v>23.4</v>
@@ -802,8 +834,8 @@
       <c r="M7" s="1">
         <v>180</v>
       </c>
-      <c r="N7" t="s">
-        <v>22</v>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="O7" s="1">
         <v>23.4</v>
@@ -849,8 +881,8 @@
       <c r="M8" s="1">
         <v>180</v>
       </c>
-      <c r="N8" t="s">
-        <v>23</v>
+      <c r="N8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="O8" s="1">
         <v>24.8</v>
@@ -896,8 +928,8 @@
       <c r="M9" s="1">
         <v>180</v>
       </c>
-      <c r="N9" t="s">
-        <v>15</v>
+      <c r="N9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="O9" s="1">
         <v>25.5</v>
@@ -943,8 +975,8 @@
       <c r="M10" s="1">
         <v>180</v>
       </c>
-      <c r="N10" t="s">
-        <v>16</v>
+      <c r="N10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="O10" s="1">
         <v>25.7</v>
@@ -990,8 +1022,8 @@
       <c r="M11" s="1">
         <v>180</v>
       </c>
-      <c r="N11" t="s">
-        <v>17</v>
+      <c r="N11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="O11" s="1">
         <v>25.7</v>
@@ -1037,8 +1069,8 @@
       <c r="M12" s="1">
         <v>180</v>
       </c>
-      <c r="N12" t="s">
-        <v>24</v>
+      <c r="N12" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O12" s="1">
         <v>26.2</v>
@@ -1084,8 +1116,8 @@
       <c r="M13" s="1">
         <v>180</v>
       </c>
-      <c r="N13" t="s">
-        <v>15</v>
+      <c r="N13" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="O13" s="1">
         <v>27.4</v>
@@ -1131,8 +1163,8 @@
       <c r="M14" s="1">
         <v>180</v>
       </c>
-      <c r="N14" t="s">
-        <v>25</v>
+      <c r="N14" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="O14" s="1">
         <v>27.4</v>
@@ -1178,8 +1210,8 @@
       <c r="M15" s="1">
         <v>180</v>
       </c>
-      <c r="N15" t="s">
-        <v>26</v>
+      <c r="N15" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O15" s="1">
         <v>28.2</v>
@@ -1225,8 +1257,8 @@
       <c r="M16" s="1">
         <v>180</v>
       </c>
-      <c r="N16" t="s">
-        <v>19</v>
+      <c r="N16" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="O16" s="1">
         <v>28.4</v>
@@ -1272,8 +1304,8 @@
       <c r="M17" s="1">
         <v>180</v>
       </c>
-      <c r="N17" t="s">
-        <v>20</v>
+      <c r="N17" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="O17" s="1">
         <v>27.8</v>
@@ -1319,8 +1351,8 @@
       <c r="M18" s="1">
         <v>180</v>
       </c>
-      <c r="N18" t="s">
-        <v>27</v>
+      <c r="N18" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="O18" s="1">
         <v>27.6</v>
@@ -1366,8 +1398,8 @@
       <c r="M19" s="1">
         <v>180</v>
       </c>
-      <c r="N19" t="s">
-        <v>22</v>
+      <c r="N19" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="O19" s="1">
         <v>26.4</v>
@@ -1413,8 +1445,8 @@
       <c r="M20" s="1">
         <v>180</v>
       </c>
-      <c r="N20" t="s">
-        <v>23</v>
+      <c r="N20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="O20" s="1">
         <v>26.2</v>
@@ -1460,8 +1492,8 @@
       <c r="M21" s="1">
         <v>180</v>
       </c>
-      <c r="N21" t="s">
-        <v>15</v>
+      <c r="N21" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="O21" s="1">
         <v>25.2</v>
@@ -1507,8 +1539,8 @@
       <c r="M22" s="1">
         <v>180</v>
       </c>
-      <c r="N22" t="s">
-        <v>16</v>
+      <c r="N22" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="O22" s="1">
         <v>25.1</v>
@@ -1554,8 +1586,8 @@
       <c r="M23" s="1">
         <v>180</v>
       </c>
-      <c r="N23" t="s">
-        <v>17</v>
+      <c r="N23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="O23" s="1">
         <v>24.8</v>
@@ -1601,8 +1633,8 @@
       <c r="M24" s="1">
         <v>180</v>
       </c>
-      <c r="N24" t="s">
-        <v>24</v>
+      <c r="N24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="O24" s="1">
         <v>23.8</v>
@@ -1648,8 +1680,8 @@
       <c r="M25" s="1">
         <v>180</v>
       </c>
-      <c r="N25" t="s">
-        <v>15</v>
+      <c r="N25" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="O25" s="1">
         <v>23.5</v>
@@ -1695,8 +1727,8 @@
       <c r="M26" s="1">
         <v>180</v>
       </c>
-      <c r="N26" t="s">
-        <v>15</v>
+      <c r="N26" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O26" s="1">
         <v>23.9</v>
@@ -1742,8 +1774,8 @@
       <c r="M27" s="1">
         <v>180</v>
       </c>
-      <c r="N27" t="s">
-        <v>18</v>
+      <c r="N27" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="O27" s="1">
         <v>24.1</v>
@@ -1789,9 +1821,6 @@
       <c r="M28" s="1">
         <v>180</v>
       </c>
-      <c r="N28" t="s">
-        <v>19</v>
-      </c>
       <c r="O28" s="1">
         <v>23.9</v>
       </c>
@@ -1836,9 +1865,6 @@
       <c r="M29" s="1">
         <v>180</v>
       </c>
-      <c r="N29" t="s">
-        <v>20</v>
-      </c>
       <c r="O29" s="1">
         <v>24.2</v>
       </c>
@@ -1883,9 +1909,6 @@
       <c r="M30" s="1">
         <v>180</v>
       </c>
-      <c r="N30" t="s">
-        <v>21</v>
-      </c>
       <c r="O30" s="1">
         <v>24.2</v>
       </c>
@@ -1930,9 +1953,6 @@
       <c r="M31" s="1">
         <v>180</v>
       </c>
-      <c r="N31" t="s">
-        <v>22</v>
-      </c>
       <c r="O31" s="1">
         <v>24.3</v>
       </c>
@@ -1977,9 +1997,6 @@
       <c r="M32" s="1">
         <v>180</v>
       </c>
-      <c r="N32" t="s">
-        <v>23</v>
-      </c>
       <c r="O32" s="1">
         <v>24.5</v>
       </c>
@@ -2024,9 +2041,6 @@
       <c r="M33" s="1">
         <v>180</v>
       </c>
-      <c r="N33" t="s">
-        <v>15</v>
-      </c>
       <c r="O33" s="1">
         <v>25.5</v>
       </c>
@@ -2071,9 +2085,6 @@
       <c r="M34" s="1">
         <v>180</v>
       </c>
-      <c r="N34" t="s">
-        <v>16</v>
-      </c>
       <c r="O34" s="1">
         <v>25.7</v>
       </c>
@@ -2118,9 +2129,6 @@
       <c r="M35" s="1">
         <v>180</v>
       </c>
-      <c r="N35" t="s">
-        <v>17</v>
-      </c>
       <c r="O35" s="1">
         <v>26.8</v>
       </c>
@@ -2165,9 +2173,6 @@
       <c r="M36" s="1">
         <v>180</v>
       </c>
-      <c r="N36" t="s">
-        <v>24</v>
-      </c>
       <c r="O36" s="1">
         <v>27</v>
       </c>
@@ -2211,9 +2216,6 @@
       </c>
       <c r="M37" s="1">
         <v>180</v>
-      </c>
-      <c r="N37" t="s">
-        <v>15</v>
       </c>
       <c r="O37" s="1">
         <v>27.4</v>

</xml_diff>